<commit_message>
changed in email template
</commit_message>
<xml_diff>
--- a/amazon-prices.xlsx
+++ b/amazon-prices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>asin</t>
   </si>
@@ -31,13 +31,34 @@
     <t>B0016H2KLS</t>
   </si>
   <si>
+    <t>Amazon.ae</t>
+  </si>
+  <si>
+    <t>AED183.16</t>
+  </si>
+  <si>
     <t>Does not import internationally</t>
   </si>
   <si>
-    <t>Amazon.ae</t>
-  </si>
-  <si>
-    <t>AED183.16</t>
+    <t>B007177NZU</t>
+  </si>
+  <si>
+    <t>AED294.58</t>
+  </si>
+  <si>
+    <t>AED295.00</t>
+  </si>
+  <si>
+    <t>AED299.00</t>
+  </si>
+  <si>
+    <t>UNER STORE</t>
+  </si>
+  <si>
+    <t>AED304.29</t>
+  </si>
+  <si>
+    <t>Ships from outside the UAE. Learn more</t>
   </si>
 </sst>
 </file>
@@ -369,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,22 +414,92 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>